<commit_message>
Added lab 8 and 9
</commit_message>
<xml_diff>
--- a/Lab 7/Assets.xlsx
+++ b/Lab 7/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://westonfamily-my.sharepoint.com/personal/matt_westonfamily_online/Documents/Book/GitHub/Learn-Microsoft-PowerApps/Lab 7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_F25DC773A252ABDACC104834B99C45145BDE58E8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98FF98F5-E779-4091-B6C9-CE40752A153B}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{973DE132-FC2E-4F45-B4D2-062FEB01F0A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54F6ED2A-B714-4A53-A040-4E25BA4EBDC9}"/>
   <x:bookViews>
-    <x:workbookView xWindow="8085" yWindow="-15870" windowWidth="25440" windowHeight="15390" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <x:si>
     <x:t>Category</x:t>
   </x:si>
@@ -65,6 +65,15 @@
     <x:t>Specification</x:t>
   </x:si>
   <x:si>
+    <x:t>Location</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Asset Photo [image]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Asset Barcode</x:t>
+  </x:si>
+  <x:si>
     <x:t>Surface Pro 6</x:t>
   </x:si>
   <x:si>
@@ -74,6 +83,9 @@
     <x:t>6D7XU_WlkLc</x:t>
   </x:si>
   <x:si>
+    <x:t>40.804000,-74.464460</x:t>
+  </x:si>
+  <x:si>
     <x:t>Surface Go</x:t>
   </x:si>
   <x:si>
@@ -90,6 +102,24 @@
   </x:si>
   <x:si>
     <x:t>jljJ2J-BMqg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>256GB HD, 8GB RAM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>320QlCiydlQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52.4804096,-2.146304</x:t>
+  </x:si>
+  <x:si>
+    <x:t>e2iK7AowT7A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52.45075178,-1.7336544</x:t>
+  </x:si>
+  <x:si>
+    <x:t>.\Assets_images\adfbff03195a43cfa06c295e07952f40.png</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -99,13 +129,20 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
+  <x:fonts count="3" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
       <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
@@ -161,7 +198,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Categories" displayName="Categories" ref="B2:D5" totalsRowShown="0">
   <x:autoFilter ref="B2:D5"/>
   <x:tableColumns count="3">
@@ -173,15 +210,18 @@
 </x:table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Assets" displayName="Assets" ref="B2:F5" totalsRowShown="0">
-  <x:autoFilter ref="B2:F5"/>
-  <x:tableColumns count="5">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Assets" displayName="Assets" ref="B2:I7" totalsRowShown="0">
+  <x:autoFilter ref="B2:I7"/>
+  <x:tableColumns count="8">
     <x:tableColumn id="1" name="Asset ID"/>
     <x:tableColumn id="2" name="Category"/>
     <x:tableColumn id="3" name="Name"/>
     <x:tableColumn id="4" name="Specification"/>
     <x:tableColumn id="5" name="__PowerAppsId__"/>
+    <x:tableColumn id="6" name="Location"/>
+    <x:tableColumn id="7" name="Asset Photo [image]"/>
+    <x:tableColumn id="8" name="Asset Barcode"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -453,7 +493,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A2:D5"/>
+  <x:dimension ref="A2:D6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
       <x:selection activeCell="C6" sqref="C6 C6:C6"/>
@@ -509,7 +549,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4">
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <x:c r="C6" s="2" t="s"/>
     </x:row>
   </x:sheetData>
@@ -528,22 +568,26 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="B2:E5"/>
+  <x:dimension ref="A2:I11"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C4" sqref="C4 C4:C4"/>
+      <x:selection activeCell="K7" sqref="K7 K7:K7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <x:col min="1" max="1" width="9.15234375" style="2" customWidth="1"/>
     <x:col min="2" max="2" width="9.921875" style="2" bestFit="1" customWidth="1"/>
     <x:col min="3" max="3" width="10.61328125" style="2" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="11.69140625" style="2" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="18.15234375" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="6" width="18.23046875" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="7" max="7" width="19.15234375" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="8" max="8" width="19.84375" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="9" max="9" width="14.84375" style="2" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <x:row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <x:c r="B2" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -559,8 +603,17 @@
       <x:c r="F2" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <x:c r="G2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <x:c r="B3" s="2" t="n">
         <x:v>1</x:v>
       </x:c>
@@ -568,16 +621,21 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D3" s="2" t="s">
-        <x:v>12</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E3" s="2" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F3" s="2" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6" x14ac:dyDescent="0.4">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s"/>
+      <x:c r="I3" s="2" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <x:c r="B4" s="2" t="n">
         <x:v>2</x:v>
       </x:c>
@@ -585,16 +643,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D4" s="2" t="s">
-        <x:v>15</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E4" s="2" t="s">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F4" s="2" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <x:c r="B5" s="2" t="n">
         <x:v>3</x:v>
       </x:c>
@@ -602,14 +663,106 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D5" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E5" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="E5" s="2" t="s">
+    </x:row>
+    <x:row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <x:c r="B6" s="2" t="n">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="F5" s="2" t="s">
-        <x:v>20</x:v>
-      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s"/>
+      <x:c r="I6" s="2" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="B7" s="2" t="s"/>
+      <x:c r="C7" s="2" t="s"/>
+      <x:c r="D7" s="2" t="s"/>
+      <x:c r="E7" s="2" t="s"/>
+      <x:c r="F7" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s"/>
+      <x:c r="K7" s="2" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="B8" s="2" t="s"/>
+      <x:c r="C8" s="2" t="s"/>
+      <x:c r="D8" s="2" t="s"/>
+      <x:c r="E8" s="2" t="s"/>
+      <x:c r="F8" s="2" t="s"/>
+      <x:c r="G8" s="2" t="s"/>
+      <x:c r="H8" s="2" t="s"/>
+      <x:c r="I8" s="2" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="B9" s="2" t="s"/>
+      <x:c r="C9" s="2" t="s"/>
+      <x:c r="D9" s="2" t="s"/>
+      <x:c r="E9" s="2" t="s"/>
+      <x:c r="F9" s="2" t="s"/>
+      <x:c r="G9" s="2" t="s"/>
+      <x:c r="H9" s="2" t="s"/>
+      <x:c r="I9" s="2" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="B10" s="2" t="s"/>
+      <x:c r="C10" s="2" t="s"/>
+      <x:c r="D10" s="2" t="s"/>
+      <x:c r="E10" s="2" t="s"/>
+      <x:c r="F10" s="2" t="s"/>
+      <x:c r="G10" s="2" t="s"/>
+      <x:c r="H10" s="2" t="s"/>
+      <x:c r="I10" s="2" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <x:c r="B11" s="2" t="s"/>
+      <x:c r="C11" s="2" t="s"/>
+      <x:c r="D11" s="2" t="s"/>
+      <x:c r="E11" s="2" t="s"/>
+      <x:c r="F11" s="2" t="s"/>
+      <x:c r="G11" s="2" t="s"/>
+      <x:c r="H11" s="2" t="s"/>
+      <x:c r="I11" s="2" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="B12" s="2" t="s"/>
+      <x:c r="C12" s="2" t="s"/>
+      <x:c r="D12" s="2" t="s"/>
+      <x:c r="E12" s="2" t="s"/>
+      <x:c r="F12" s="2" t="s"/>
+      <x:c r="G12" s="2" t="s"/>
+      <x:c r="H12" s="2" t="s"/>
+      <x:c r="I12" s="2" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>